<commit_message>
get rid of Context file
</commit_message>
<xml_diff>
--- a/ExcelReader/TestData/BookStore1.xlsx
+++ b/ExcelReader/TestData/BookStore1.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myroslava_Konko\Source\Mentoring\Hometasks\ExcelReader\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -48,36 +40,90 @@
     <t>Total Sold Price</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>J.K. Rowling</t>
   </si>
   <si>
     <t>Harry Potter and the Cursed Child</t>
   </si>
   <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Fantasy</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Fantastic Beasts And Where To Find Them</t>
   </si>
   <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>J.R. Tolkien</t>
   </si>
   <si>
     <t>Silmarillion</t>
   </si>
   <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Lord Of The Ring: Two Towers</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Stephen King</t>
   </si>
   <si>
     <t>Shining</t>
   </si>
   <si>
+    <t>80</t>
+  </si>
+  <si>
     <t>Horror</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Ray Bradbury</t>
   </si>
   <si>
@@ -87,32 +133,53 @@
     <t>Dystopian  Fiction</t>
   </si>
   <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>Dandelion Wine</t>
   </si>
   <si>
+    <t>120</t>
+  </si>
+  <si>
     <t>Fiction</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>It</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>Herman Mellwill</t>
   </si>
   <si>
     <t>Mobi Dick</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
+    <t>50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -120,28 +187,37 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="11"/>
       <name val="Menlo"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -154,35 +230,44 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,85 +276,25 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FFE38400"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffe38400"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -461,17 +486,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -490,19 +515,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -520,7 +545,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -546,7 +571,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -572,7 +597,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -598,7 +623,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -624,7 +649,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -650,7 +675,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -676,7 +701,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -702,7 +727,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -728,7 +753,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -741,32 +766,26 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -785,7 +804,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -811,7 +830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -837,7 +856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -863,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -967,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -993,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1032,15 +1051,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1054,7 +1067,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1073,19 +1086,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1103,7 +1116,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1129,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1181,7 +1194,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1207,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1233,7 +1246,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1259,7 +1272,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1285,7 +1298,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1311,7 +1324,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1324,345 +1337,338 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="20.140625" style="1" customWidth="1"/>
-    <col min="10" max="256" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1719" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1719" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1719" style="1" customWidth="1"/>
+    <col min="10" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.100000000000001" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="17.1" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" t="s" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="5">
-        <v>75</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="C2" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5">
+        <f>D2*H2</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5">
+        <f>D3*H3</f>
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="I4" s="5">
+        <f>D4*H4</f>
+        <v>22400</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5">
-        <v>100</v>
-      </c>
-      <c r="I2" s="5">
-        <f t="shared" ref="I2:I10" si="0">D2*H2</f>
-        <v>7500</v>
+      <c r="B5" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5">
+        <f>D5*H5</f>
+        <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>110</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>90</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" si="0"/>
-        <v>9900</v>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="I6" s="5">
+        <f>D6*H6</f>
+        <v>16000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I7" s="5">
+        <f>D7*H7</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="I8" s="5">
+        <f>D8*H8</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5">
-        <v>160</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
-        <v>140</v>
-      </c>
-      <c r="I4" s="5">
-        <f t="shared" si="0"/>
+      <c r="F9" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="I9" s="5">
+        <f>D9*H9</f>
         <v>22400</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="5">
-        <v>100</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5">
-        <v>15</v>
-      </c>
-      <c r="H5" s="5">
-        <v>200</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" si="0"/>
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5">
-        <v>80</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>200</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" si="0"/>
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5">
-        <v>80</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="5">
-        <v>5</v>
-      </c>
-      <c r="H7" s="5">
-        <v>180</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>14400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="5">
-        <v>120</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="5">
-        <v>10</v>
-      </c>
-      <c r="H8" s="5">
-        <v>150</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="0"/>
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="5">
-        <v>160</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5">
-        <v>140</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="0"/>
-        <v>22400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5">
-        <v>110</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="5">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5">
-        <v>50</v>
+      <c r="F10" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>52</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="0"/>
+        <f>D10*H10</f>
         <v>5500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>